<commit_message>
before removing manual model
</commit_message>
<xml_diff>
--- a/Data_generator_template.xlsx
+++ b/Data_generator_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Crosstalk\Machine_Learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Crosstalk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE6D2BA-52BA-4C26-A386-60B83529F6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4983BCC-C67F-423B-90BE-13571EA87408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{0CBD37D8-874B-478E-990B-362705820D59}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CBD37D8-874B-478E-990B-362705820D59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Shots</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>Gamma_1</t>
+  </si>
+  <si>
+    <t>Gamma_2</t>
   </si>
 </sst>
 </file>
@@ -111,9 +117,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,21 +455,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C56A25-D89C-4ABA-83AE-C678C1F4EE43}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="16.625" customWidth="1"/>
-    <col min="10" max="10" width="86.5" customWidth="1"/>
+    <col min="1" max="2" width="16.59765625" customWidth="1"/>
+    <col min="3" max="3" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="16.59765625" customWidth="1"/>
+    <col min="12" max="12" width="127.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -476,28 +483,34 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -511,30 +524,36 @@
         <v>10000</v>
       </c>
       <c r="E2" s="1">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1">
         <v>0</v>
       </c>
-      <c r="J2" s="1" t="str">
-        <f>"Qubits_"&amp;A2&amp;"_Lines_"&amp;B2&amp;"_TS_"&amp;C2&amp;"_Shots_"&amp;D2&amp;"_MeanDecay_"&amp;E2&amp;"_MeanW_"&amp;F2&amp;"_MeanJ_"&amp;G2&amp;"_Std_"&amp;H2&amp;"_Correlations_"&amp;I2&amp;"_"&amp;K2</f>
-        <v>Qubits_2_Lines_10_TS_2_Shots_10000_MeanDecay_1_MeanW_0_MeanJ_0_Std_1_Correlations_0_1</v>
+      <c r="J2" s="1">
+        <v>1</v>
       </c>
       <c r="K2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="str">
+        <f>"Qubits_"&amp;A2&amp;"_Lines_"&amp;B2&amp;"_TS_"&amp;C2&amp;"_Shots_"&amp;D2&amp;"_MeanDecay_"&amp;G2&amp;"G&amp;Gamma_1 "&amp;E2&amp;"Gamma_2 "&amp;F2&amp;"_MeanW_"&amp;H2&amp;"_MeanJ_"&amp;I2&amp;"_Std_"&amp;J2&amp;"_Correlations_"&amp;K2&amp;"_"&amp;M2</f>
+        <v>Qubits_2_Lines_10_TS_2_Shots_10000_MeanDecay_1G&amp;Gamma_1 0.0001Gamma_2 0.0001_MeanW_0_MeanJ_0_Std_1_Correlations_0_1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -547,66 +566,161 @@
         <v>10000</v>
       </c>
       <c r="E3" s="1">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
       <c r="F3" s="1">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
       </c>
-      <c r="J3" s="1" t="str">
-        <f t="shared" ref="J3:J16" si="0">"Qubits_"&amp;A3&amp;"_Lines_"&amp;B3&amp;"_TS_"&amp;C3&amp;"_Shots_"&amp;D3&amp;"_MeanDecay_"&amp;E3&amp;"_MeanW_"&amp;F3&amp;"_MeanJ_"&amp;G3&amp;"_Std_"&amp;H3&amp;"_Correlations_"&amp;I3&amp;"_"&amp;K3</f>
-        <v>Qubits_2_Lines_10_TS_2_Shots_10000_MeanDecay_1_MeanW_0_MeanJ_0_Std_1_Correlations_0_2</v>
+      <c r="J3" s="1">
+        <v>1</v>
       </c>
       <c r="K3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="L3" s="1" t="str">
+        <f>"Qubits_"&amp;A3&amp;"_Lines_"&amp;B3&amp;"_TS_"&amp;C3&amp;"_Shots_"&amp;D3&amp;"_MeanDecay_"&amp;G3&amp;"G&amp;Gamma_1 "&amp;E3&amp;"Gamma_2 "&amp;F3&amp;"_MeanW_"&amp;H3&amp;"_MeanJ_"&amp;I3&amp;"_Std_"&amp;J3&amp;"_Correlations_"&amp;K3&amp;"_"&amp;M3</f>
+        <v>Qubits_2_Lines_10_TS_2_Shots_10000_MeanDecay_1G&amp;Gamma_1 0.001Gamma_2 0.0001_MeanW_0_MeanJ_0_Std_1_Correlations_0_1</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f>"Qubits_"&amp;A4&amp;"_Lines_"&amp;B4&amp;"_TS_"&amp;C4&amp;"_Shots_"&amp;D4&amp;"_MeanDecay_"&amp;G4&amp;"G&amp;Gamma_1 "&amp;E4&amp;"Gamma_2 "&amp;F4&amp;"_MeanW_"&amp;H4&amp;"_MeanJ_"&amp;I4&amp;"_Std_"&amp;J4&amp;"_Correlations_"&amp;K4&amp;"_"&amp;M4</f>
+        <v>Qubits_2_Lines_10_TS_2_Shots_10000_MeanDecay_1G&amp;Gamma_1 0.01Gamma_2 0.0001_MeanW_0_MeanJ_0_Std_1_Correlations_0_1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1" t="str">
+        <f>"Qubits_"&amp;A5&amp;"_Lines_"&amp;B5&amp;"_TS_"&amp;C5&amp;"_Shots_"&amp;D5&amp;"_MeanDecay_"&amp;G5&amp;"G&amp;Gamma_1 "&amp;E5&amp;"Gamma_2 "&amp;F5&amp;"_MeanW_"&amp;H5&amp;"_MeanJ_"&amp;I5&amp;"_Std_"&amp;J5&amp;"_Correlations_"&amp;K5&amp;"_"&amp;M5</f>
+        <v>Qubits_2_Lines_10_TS_2_Shots_10000_MeanDecay_1G&amp;Gamma_1 0.1Gamma_2 0.0001_MeanW_0_MeanJ_0_Std_1_Correlations_0_1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="str">
+        <f>"Qubits_"&amp;A6&amp;"_Lines_"&amp;B6&amp;"_TS_"&amp;C6&amp;"_Shots_"&amp;D6&amp;"_MeanDecay_"&amp;G6&amp;"G&amp;Gamma_1 "&amp;E6&amp;"Gamma_2 "&amp;F6&amp;"_MeanW_"&amp;H6&amp;"_MeanJ_"&amp;I6&amp;"_Std_"&amp;J6&amp;"_Correlations_"&amp;K6&amp;"_"&amp;M6</f>
+        <v>Qubits_2_Lines_10_TS_2_Shots_10000_MeanDecay_1G&amp;Gamma_1 1Gamma_2 0.0001_MeanW_0_MeanJ_0_Std_1_Correlations_0_1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -617,8 +731,10 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -629,8 +745,10 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -641,8 +759,10 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -653,8 +773,10 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -665,8 +787,10 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -677,8 +801,10 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -689,8 +815,10 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -701,8 +829,11 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -713,31 +844,22 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>